<commit_message>
Algoritmos y Datasets completos
</commit_message>
<xml_diff>
--- a/Tarea 1/Algoritmos De Ordenamiento/Resultados/ComparacionAlgoritmosDeOrdenamiento.xlsx
+++ b/Tarea 1/Algoritmos De Ordenamiento/Resultados/ComparacionAlgoritmosDeOrdenamiento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Universidad\2024\Segundo Semestre\Algoco\Tareas\Tarea 1\Algoritmos De Ordenamiento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gomez\OneDrive\Documentos\0GitHub\Tareas_Algoco_GitHub\Tarea 1\Algoritmos De Ordenamiento\Resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D765E42E-710D-4D81-A16E-5BB019EC6741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D566CDAA-E15B-4DBB-8D96-41761CB46E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{79BE7122-2C17-4AAB-9D74-077BE3265EBA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="58">
   <si>
     <t>Tamaño</t>
   </si>
@@ -209,7 +209,7 @@
     <t>Cpu: AMD Ryzen 3 3200G (3.6GHz) (4 Núcleos)</t>
   </si>
   <si>
-    <t>Caso no probado</t>
+    <t>Tiempo excedido</t>
   </si>
 </sst>
 </file>
@@ -217,7 +217,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -298,30 +298,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C1468D0-3977-4575-8573-BAFE8087FD9A}">
   <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,37 +667,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="12"/>
+      <c r="D1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="J1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="P1" s="3" t="s">
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="P1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="7"/>
+      <c r="B2" s="12"/>
       <c r="D2" s="2" t="s">
         <v>49</v>
       </c>
@@ -746,30 +745,30 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="D3" s="5">
+      <c r="B3" s="12"/>
+      <c r="D3" s="3">
         <f>AVERAGE(D12:D15)</f>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="5">
         <f>AVERAGE(I12:I15)</f>
         <v>7.8500000000000011E-3</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="5">
         <f>AVERAGE(N12:N15)</f>
         <v>8.4999999999999995E-4</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="5">
         <f>AVERAGE(S12:S15)</f>
         <v>1.475E-3</v>
       </c>
       <c r="H3" s="2">
         <v>10</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="3">
         <f>D36</f>
         <v>2.0000000000000001E-4</v>
       </c>
@@ -777,7 +776,7 @@
         <f>I36</f>
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="5">
         <f>N36</f>
         <v>1E-3</v>
       </c>
@@ -788,7 +787,7 @@
       <c r="N3" s="2">
         <v>10</v>
       </c>
-      <c r="P3" s="13">
+      <c r="P3" s="3">
         <f>D42</f>
         <v>5.0000000000000001E-4</v>
       </c>
@@ -809,28 +808,28 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="D4" s="9">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="D4" s="5">
         <f>AVERAGE(D16:D19)</f>
         <v>8.6750000000000004E-3</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="5">
         <f>AVERAGE(I16:I19)</f>
         <v>7.947499999999999E-2</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="8">
         <f>AVERAGE(N16:N19)</f>
         <v>8.0250000000000009E-3</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="5">
         <f>AVERAGE(S16:S19)</f>
         <v>8.4749999999999999E-3</v>
       </c>
       <c r="H4" s="2">
         <v>100</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="3">
         <f t="shared" ref="J4:J8" si="0">D37</f>
         <v>5.9999999999999995E-4</v>
       </c>
@@ -857,11 +856,11 @@
         <f t="shared" ref="Q4:Q8" si="5">I43</f>
         <v>7.5800000000000006E-2</v>
       </c>
-      <c r="R4" s="9">
+      <c r="R4" s="5">
         <f t="shared" ref="R4:R8" si="6">N43</f>
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="S4" s="13">
+      <c r="S4" s="3">
         <f t="shared" ref="S4:S8" si="7">S43</f>
         <v>4.4000000000000003E-3</v>
       </c>
@@ -870,7 +869,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D5" s="9">
+      <c r="D5" s="5">
         <f>AVERAGE(D20:D23)</f>
         <v>0.72450000000000003</v>
       </c>
@@ -878,18 +877,18 @@
         <f>AVERAGE(I20:I23)</f>
         <v>0.78810000000000002</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="5">
         <f>AVERAGE(N20:N23)</f>
         <v>0.13485</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="8">
         <f>AVERAGE(S20:S23)</f>
         <v>0.10062499999999999</v>
       </c>
       <c r="H5" s="2">
         <v>1000</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="3">
         <f t="shared" si="0"/>
         <v>3.5999999999999999E-3</v>
       </c>
@@ -920,7 +919,7 @@
         <f t="shared" si="6"/>
         <v>2.7966000000000002</v>
       </c>
-      <c r="S5" s="13">
+      <c r="S5" s="3">
         <f t="shared" si="7"/>
         <v>3.5299999999999998E-2</v>
       </c>
@@ -929,26 +928,26 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D6" s="9">
+      <c r="D6" s="5">
         <f>AVERAGE(D24:D27)</f>
         <v>85.985024999999993</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="5">
         <f>AVERAGE(I24:I27)</f>
         <v>9.6294249999999995</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="5">
         <f>AVERAGE(N24:N27)</f>
         <v>1.6503999999999999</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="8">
         <f>AVERAGE(S24:S27)</f>
         <v>1.3605</v>
       </c>
       <c r="H6" s="2">
         <v>10000</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="3">
         <f t="shared" si="0"/>
         <v>4.0500000000000001E-2</v>
       </c>
@@ -960,7 +959,7 @@
         <f t="shared" si="2"/>
         <v>486.09960000000001</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="5">
         <f t="shared" si="3"/>
         <v>0.56399999999999995</v>
       </c>
@@ -979,7 +978,7 @@
         <f t="shared" si="6"/>
         <v>309.66820000000001</v>
       </c>
-      <c r="S6" s="13">
+      <c r="S6" s="3">
         <f t="shared" si="7"/>
         <v>0.46129999999999999</v>
       </c>
@@ -992,7 +991,7 @@
         <f>AVERAGE(D28:D31)</f>
         <v>7530.2647000000006</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="5">
         <f>AVERAGE(I28:I31)</f>
         <v>120.44595000000001</v>
       </c>
@@ -1000,14 +999,14 @@
         <f>AVERAGE(N28:N31)</f>
         <v>21.031199999999998</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="8">
         <f>AVERAGE(S28:S31)</f>
         <v>18.091024999999998</v>
       </c>
       <c r="H7" s="2">
         <v>100000</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="3">
         <f t="shared" si="0"/>
         <v>0.61029999999999995</v>
       </c>
@@ -1038,7 +1037,7 @@
         <f t="shared" si="6"/>
         <v>28754.259099999999</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="3">
         <f t="shared" si="7"/>
         <v>6.5110999999999999</v>
       </c>
@@ -1050,22 +1049,22 @@
       <c r="D8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="5">
         <f>AVERAGE(I32:I35)</f>
         <v>3028.7257250000002</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="5">
         <f>AVERAGE(N32:N35)</f>
         <v>237.59915000000001</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="8">
         <f>AVERAGE(S32:S35)</f>
         <v>236.78722499999998</v>
       </c>
       <c r="H8" s="2">
         <v>1000000</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="3">
         <f t="shared" si="0"/>
         <v>5.9401000000000002</v>
       </c>
@@ -1073,9 +1072,8 @@
         <f t="shared" si="1"/>
         <v>2973.2116000000001</v>
       </c>
-      <c r="L8" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Caso no probado</v>
+      <c r="L8" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="3"/>
@@ -1084,19 +1082,17 @@
       <c r="N8" s="2">
         <v>1000000</v>
       </c>
-      <c r="P8" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>Caso no probado</v>
+      <c r="P8" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="Q8" s="2">
         <f t="shared" si="5"/>
         <v>2566.0655000000002</v>
       </c>
-      <c r="R8" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>Caso no probado</v>
-      </c>
-      <c r="S8" s="2">
+      <c r="R8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="S8" s="3">
         <f t="shared" si="7"/>
         <v>63.661099999999998</v>
       </c>
@@ -1105,30 +1101,30 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="H10" s="4" t="s">
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="H10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="M10" s="4" t="s">
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="M10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="R10" s="4" t="s">
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="R10" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
@@ -1381,202 +1377,202 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C16" s="10">
+      <c r="C16" s="6">
         <v>100</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="7">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" s="10">
+      <c r="F16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="6">
         <v>100</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="6">
         <v>7.3899999999999993E-2</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K16" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M16" s="10">
+      <c r="K16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M16" s="6">
         <v>100</v>
       </c>
-      <c r="N16" s="10">
+      <c r="N16" s="6">
         <v>7.6E-3</v>
       </c>
-      <c r="O16" s="10" t="s">
+      <c r="O16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P16" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="R16" s="10">
+      <c r="P16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R16" s="6">
         <v>100</v>
       </c>
-      <c r="S16" s="10">
+      <c r="S16" s="6">
         <v>8.6E-3</v>
       </c>
-      <c r="T16" s="10" t="s">
+      <c r="T16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="U16" s="10" t="s">
+      <c r="U16" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C17" s="10">
+      <c r="C17" s="6">
         <v>100</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="7">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="10">
+      <c r="F17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="6">
         <v>100</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="6">
         <v>7.3800000000000004E-2</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M17" s="10">
+      <c r="K17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M17" s="6">
         <v>100</v>
       </c>
-      <c r="N17" s="10">
+      <c r="N17" s="6">
         <v>8.6E-3</v>
       </c>
-      <c r="O17" s="10" t="s">
+      <c r="O17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="P17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="R17" s="10">
+      <c r="P17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R17" s="6">
         <v>100</v>
       </c>
-      <c r="S17" s="10">
+      <c r="S17" s="6">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="T17" s="10" t="s">
+      <c r="T17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="U17" s="10" t="s">
+      <c r="U17" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C18" s="10">
+      <c r="C18" s="6">
         <v>100</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="6">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H18" s="10">
+      <c r="F18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="6">
         <v>100</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="6">
         <v>9.2899999999999996E-2</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K18" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M18" s="10">
+      <c r="K18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M18" s="6">
         <v>100</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="7">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="O18" s="10" t="s">
+      <c r="O18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P18" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="R18" s="10">
+      <c r="P18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R18" s="6">
         <v>100</v>
       </c>
-      <c r="S18" s="11">
+      <c r="S18" s="7">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="T18" s="10" t="s">
+      <c r="T18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="U18" s="10" t="s">
+      <c r="U18" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="19" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C19" s="10">
+      <c r="C19" s="6">
         <v>100</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="6">
         <v>8.6E-3</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H19" s="10">
+      <c r="F19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="6">
         <v>100</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="6">
         <v>7.7299999999999994E-2</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M19" s="10">
+      <c r="K19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" s="6">
         <v>100</v>
       </c>
-      <c r="N19" s="10">
+      <c r="N19" s="6">
         <v>7.9000000000000008E-3</v>
       </c>
-      <c r="O19" s="10" t="s">
+      <c r="O19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="P19" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="R19" s="10">
+      <c r="P19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R19" s="6">
         <v>100</v>
       </c>
-      <c r="S19" s="10">
+      <c r="S19" s="6">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="T19" s="10" t="s">
+      <c r="T19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="U19" s="10" t="s">
+      <c r="U19" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1596,7 +1592,7 @@
       <c r="H20" s="1">
         <v>1000</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="4">
         <v>0.871</v>
       </c>
       <c r="J20" s="1" t="s">
@@ -1620,7 +1616,7 @@
       <c r="R20" s="1">
         <v>1000</v>
       </c>
-      <c r="S20" s="6">
+      <c r="S20" s="4">
         <v>0.10100000000000001</v>
       </c>
       <c r="T20" s="1" t="s">
@@ -1781,202 +1777,202 @@
       </c>
     </row>
     <row r="24" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C24" s="10">
+      <c r="C24" s="6">
         <v>10000</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="6">
         <v>87.817899999999995</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H24" s="10">
+      <c r="F24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="6">
         <v>10000</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="6">
         <v>9.6961999999999993</v>
       </c>
-      <c r="J24" s="10" t="s">
+      <c r="J24" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M24" s="10">
+      <c r="K24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M24" s="6">
         <v>10000</v>
       </c>
-      <c r="N24" s="10">
+      <c r="N24" s="6">
         <v>1.5823</v>
       </c>
-      <c r="O24" s="10" t="s">
+      <c r="O24" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="P24" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="R24" s="10">
+      <c r="P24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R24" s="6">
         <v>10000</v>
       </c>
-      <c r="S24" s="10">
+      <c r="S24" s="6">
         <v>1.2679</v>
       </c>
-      <c r="T24" s="10" t="s">
+      <c r="T24" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="U24" s="10" t="s">
+      <c r="U24" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C25" s="10">
+      <c r="C25" s="6">
         <v>10000</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="6">
         <v>85.161299999999997</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H25" s="10">
+      <c r="F25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" s="6">
         <v>10000</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="6">
         <v>9.0953999999999997</v>
       </c>
-      <c r="J25" s="10" t="s">
+      <c r="J25" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M25" s="10">
+      <c r="K25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M25" s="6">
         <v>10000</v>
       </c>
-      <c r="N25" s="10">
+      <c r="N25" s="6">
         <v>1.5737000000000001</v>
       </c>
-      <c r="O25" s="10" t="s">
+      <c r="O25" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="P25" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="R25" s="10">
+      <c r="P25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R25" s="6">
         <v>10000</v>
       </c>
-      <c r="S25" s="10">
+      <c r="S25" s="6">
         <v>1.3394999999999999</v>
       </c>
-      <c r="T25" s="10" t="s">
+      <c r="T25" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="U25" s="10" t="s">
+      <c r="U25" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="26" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C26" s="10">
+      <c r="C26" s="6">
         <v>10000</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="6">
         <v>88.473500000000001</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H26" s="10">
+      <c r="F26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" s="6">
         <v>10000</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26" s="6">
         <v>10.792299999999999</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="J26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K26" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M26" s="10">
+      <c r="K26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M26" s="6">
         <v>10000</v>
       </c>
-      <c r="N26" s="10">
+      <c r="N26" s="6">
         <v>2.0004</v>
       </c>
-      <c r="O26" s="10" t="s">
+      <c r="O26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P26" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="R26" s="10">
+      <c r="P26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R26" s="6">
         <v>10000</v>
       </c>
-      <c r="S26" s="10">
+      <c r="S26" s="6">
         <v>1.5327</v>
       </c>
-      <c r="T26" s="10" t="s">
+      <c r="T26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U26" s="10" t="s">
+      <c r="U26" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C27" s="10">
+      <c r="C27" s="6">
         <v>10000</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="6">
         <v>82.487399999999994</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H27" s="10">
+      <c r="F27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" s="6">
         <v>10000</v>
       </c>
-      <c r="I27" s="10">
+      <c r="I27" s="6">
         <v>8.9337999999999997</v>
       </c>
-      <c r="J27" s="10" t="s">
+      <c r="J27" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K27" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M27" s="10">
+      <c r="K27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M27" s="6">
         <v>10000</v>
       </c>
-      <c r="N27" s="10">
+      <c r="N27" s="6">
         <v>1.4452</v>
       </c>
-      <c r="O27" s="10" t="s">
+      <c r="O27" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P27" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="R27" s="10">
+      <c r="P27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R27" s="6">
         <v>10000</v>
       </c>
-      <c r="S27" s="10">
+      <c r="S27" s="6">
         <v>1.3019000000000001</v>
       </c>
-      <c r="T27" s="10" t="s">
+      <c r="T27" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="U27" s="10" t="s">
+      <c r="U27" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2017,10 +2013,10 @@
       <c r="P28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="R28" s="14">
+      <c r="R28" s="9">
         <v>100000</v>
       </c>
-      <c r="S28" s="6">
+      <c r="S28" s="4">
         <v>17.207000000000001</v>
       </c>
       <c r="T28" s="1" t="s">
@@ -2058,7 +2054,7 @@
       <c r="M29" s="1">
         <v>100000</v>
       </c>
-      <c r="N29" s="6">
+      <c r="N29" s="4">
         <v>21.332000000000001</v>
       </c>
       <c r="O29" s="1" t="s">
@@ -2158,7 +2154,7 @@
       <c r="M31" s="1">
         <v>100000</v>
       </c>
-      <c r="N31" s="6">
+      <c r="N31" s="4">
         <v>18.841000000000001</v>
       </c>
       <c r="O31" s="1" t="s">
@@ -2181,202 +2177,202 @@
       </c>
     </row>
     <row r="32" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C32" s="10">
+      <c r="C32" s="6">
         <v>1000000</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H32" s="10">
+      <c r="F32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H32" s="6">
         <v>1000000</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I32" s="6">
         <v>3054.9023000000002</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="J32" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K32" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M32" s="10">
+      <c r="K32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M32" s="6">
         <v>1000000</v>
       </c>
-      <c r="N32" s="10">
+      <c r="N32" s="6">
         <v>247.58959999999999</v>
       </c>
-      <c r="O32" s="10" t="s">
+      <c r="O32" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="P32" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="R32" s="10">
+      <c r="P32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R32" s="6">
         <v>1000000</v>
       </c>
-      <c r="S32" s="10">
+      <c r="S32" s="6">
         <v>222.6403</v>
       </c>
-      <c r="T32" s="10" t="s">
+      <c r="T32" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="U32" s="10" t="s">
+      <c r="U32" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="33" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C33" s="10">
+      <c r="C33" s="6">
         <v>1000000</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F33" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H33" s="10">
+      <c r="F33" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" s="6">
         <v>1000000</v>
       </c>
-      <c r="I33" s="10">
+      <c r="I33" s="6">
         <v>2094.6669000000002</v>
       </c>
-      <c r="J33" s="10" t="s">
+      <c r="J33" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K33" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M33" s="10">
+      <c r="K33" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M33" s="6">
         <v>1000000</v>
       </c>
-      <c r="N33" s="10">
+      <c r="N33" s="6">
         <v>240.2713</v>
       </c>
-      <c r="O33" s="10" t="s">
+      <c r="O33" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="P33" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="R33" s="10">
+      <c r="P33" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R33" s="6">
         <v>1000000</v>
       </c>
-      <c r="S33" s="10">
+      <c r="S33" s="6">
         <v>220.91319999999999</v>
       </c>
-      <c r="T33" s="10" t="s">
+      <c r="T33" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="U33" s="10" t="s">
+      <c r="U33" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="34" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C34" s="10">
+      <c r="C34" s="6">
         <v>1000000</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F34" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H34" s="10">
+      <c r="F34" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H34" s="6">
         <v>1000000</v>
       </c>
-      <c r="I34" s="10">
+      <c r="I34" s="6">
         <v>3161.1239</v>
       </c>
-      <c r="J34" s="10" t="s">
+      <c r="J34" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K34" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M34" s="10">
+      <c r="K34" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M34" s="6">
         <v>1000000</v>
       </c>
-      <c r="N34" s="10">
+      <c r="N34" s="6">
         <v>226.21279999999999</v>
       </c>
-      <c r="O34" s="10" t="s">
+      <c r="O34" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P34" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="R34" s="10">
+      <c r="P34" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R34" s="6">
         <v>1000000</v>
       </c>
-      <c r="S34" s="10">
+      <c r="S34" s="6">
         <v>277.19209999999998</v>
       </c>
-      <c r="T34" s="10" t="s">
+      <c r="T34" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="U34" s="10" t="s">
+      <c r="U34" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="35" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C35" s="10">
+      <c r="C35" s="6">
         <v>1000000</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H35" s="10">
+      <c r="F35" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H35" s="6">
         <v>1000000</v>
       </c>
-      <c r="I35" s="10">
+      <c r="I35" s="6">
         <v>3804.2098000000001</v>
       </c>
-      <c r="J35" s="10" t="s">
+      <c r="J35" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="K35" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M35" s="10">
+      <c r="K35" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M35" s="6">
         <v>1000000</v>
       </c>
-      <c r="N35" s="10">
+      <c r="N35" s="6">
         <v>236.3229</v>
       </c>
-      <c r="O35" s="10" t="s">
+      <c r="O35" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="P35" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="R35" s="10">
+      <c r="P35" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R35" s="6">
         <v>1000000</v>
       </c>
-      <c r="S35" s="10">
+      <c r="S35" s="6">
         <v>226.4033</v>
       </c>
-      <c r="T35" s="10" t="s">
+      <c r="T35" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="U35" s="10" t="s">
+      <c r="U35" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2408,7 +2404,7 @@
       <c r="M36" s="1">
         <v>10</v>
       </c>
-      <c r="N36" s="6">
+      <c r="N36" s="4">
         <v>1E-3</v>
       </c>
       <c r="O36" s="1" t="s">
@@ -2570,7 +2566,7 @@
       <c r="R39" s="1">
         <v>10000</v>
       </c>
-      <c r="S39" s="6">
+      <c r="S39" s="4">
         <v>0.56399999999999995</v>
       </c>
       <c r="T39" s="1" t="s">
@@ -2681,302 +2677,302 @@
       </c>
     </row>
     <row r="42" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C42" s="10">
+      <c r="C42" s="6">
         <v>10</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="6">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H42" s="10">
+      <c r="H42" s="6">
         <v>10</v>
       </c>
-      <c r="I42" s="10">
+      <c r="I42" s="6">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="J42" s="10" t="s">
+      <c r="J42" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K42" s="10" t="s">
+      <c r="K42" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M42" s="10">
+      <c r="M42" s="6">
         <v>10</v>
       </c>
-      <c r="N42" s="10">
+      <c r="N42" s="6">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="O42" s="10" t="s">
+      <c r="O42" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="P42" s="10" t="s">
+      <c r="P42" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="R42" s="10">
+      <c r="R42" s="6">
         <v>10</v>
       </c>
-      <c r="S42" s="10">
+      <c r="S42" s="6">
         <v>1.4E-3</v>
       </c>
-      <c r="T42" s="10" t="s">
+      <c r="T42" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="U42" s="10" t="s">
+      <c r="U42" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="43" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C43" s="10">
+      <c r="C43" s="6">
         <v>100</v>
       </c>
-      <c r="D43" s="10">
+      <c r="D43" s="6">
         <v>1.54E-2</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F43" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H43" s="10">
+      <c r="H43" s="6">
         <v>100</v>
       </c>
-      <c r="I43" s="10">
+      <c r="I43" s="6">
         <v>7.5800000000000006E-2</v>
       </c>
-      <c r="J43" s="10" t="s">
+      <c r="J43" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="K43" s="10" t="s">
+      <c r="K43" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M43" s="10">
+      <c r="M43" s="6">
         <v>100</v>
       </c>
-      <c r="N43" s="11">
+      <c r="N43" s="7">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="O43" s="10" t="s">
+      <c r="O43" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="P43" s="10" t="s">
+      <c r="P43" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="R43" s="10">
+      <c r="R43" s="6">
         <v>100</v>
       </c>
-      <c r="S43" s="10">
+      <c r="S43" s="6">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="T43" s="10" t="s">
+      <c r="T43" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="U43" s="10" t="s">
+      <c r="U43" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="44" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C44" s="10">
+      <c r="C44" s="6">
         <v>1000</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="6">
         <v>1.7547999999999999</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H44" s="10">
+      <c r="H44" s="6">
         <v>1000</v>
       </c>
-      <c r="I44" s="10">
+      <c r="I44" s="6">
         <v>1.2867</v>
       </c>
-      <c r="J44" s="10" t="s">
+      <c r="J44" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K44" s="10" t="s">
+      <c r="K44" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="10">
+      <c r="M44" s="6">
         <v>1000</v>
       </c>
-      <c r="N44" s="10">
+      <c r="N44" s="6">
         <v>2.7966000000000002</v>
       </c>
-      <c r="O44" s="10" t="s">
+      <c r="O44" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="P44" s="10" t="s">
+      <c r="P44" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="R44" s="10">
+      <c r="R44" s="6">
         <v>1000</v>
       </c>
-      <c r="S44" s="10">
+      <c r="S44" s="6">
         <v>3.5299999999999998E-2</v>
       </c>
-      <c r="T44" s="10" t="s">
+      <c r="T44" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="U44" s="10" t="s">
+      <c r="U44" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="45" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C45" s="10">
+      <c r="C45" s="6">
         <v>10000</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D45" s="6">
         <v>173.40459999999999</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="F45" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H45" s="10">
+      <c r="H45" s="6">
         <v>10000</v>
       </c>
-      <c r="I45" s="10">
+      <c r="I45" s="6">
         <v>8.8992000000000004</v>
       </c>
-      <c r="J45" s="10" t="s">
+      <c r="J45" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K45" s="10" t="s">
+      <c r="K45" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M45" s="10">
+      <c r="M45" s="6">
         <v>10000</v>
       </c>
-      <c r="N45" s="10">
+      <c r="N45" s="6">
         <v>309.66820000000001</v>
       </c>
-      <c r="O45" s="10" t="s">
+      <c r="O45" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="P45" s="10" t="s">
+      <c r="P45" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="R45" s="10">
+      <c r="R45" s="6">
         <v>10000</v>
       </c>
-      <c r="S45" s="10">
+      <c r="S45" s="6">
         <v>0.46129999999999999</v>
       </c>
-      <c r="T45" s="10" t="s">
+      <c r="T45" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="U45" s="10" t="s">
+      <c r="U45" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="46" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C46" s="10">
+      <c r="C46" s="6">
         <v>100000</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="6">
         <v>14647.0414</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H46" s="10">
+      <c r="H46" s="6">
         <v>100000</v>
       </c>
-      <c r="I46" s="10">
+      <c r="I46" s="6">
         <v>99.658199999999994</v>
       </c>
-      <c r="J46" s="10" t="s">
+      <c r="J46" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K46" s="10" t="s">
+      <c r="K46" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M46" s="10">
+      <c r="M46" s="6">
         <v>100000</v>
       </c>
-      <c r="N46" s="10">
+      <c r="N46" s="6">
         <v>28754.259099999999</v>
       </c>
-      <c r="O46" s="10" t="s">
+      <c r="O46" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="P46" s="10" t="s">
+      <c r="P46" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="R46" s="10">
+      <c r="R46" s="6">
         <v>100000</v>
       </c>
-      <c r="S46" s="10">
+      <c r="S46" s="6">
         <v>6.5110999999999999</v>
       </c>
-      <c r="T46" s="10" t="s">
+      <c r="T46" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="U46" s="10" t="s">
+      <c r="U46" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C47" s="10">
+      <c r="C47" s="6">
         <v>1000000</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E47" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F47" s="10" t="s">
+      <c r="F47" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H47" s="10">
+      <c r="H47" s="6">
         <v>1000000</v>
       </c>
-      <c r="I47" s="10">
+      <c r="I47" s="6">
         <v>2566.0655000000002</v>
       </c>
-      <c r="J47" s="10" t="s">
+      <c r="J47" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K47" s="10" t="s">
+      <c r="K47" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M47" s="10">
+      <c r="M47" s="6">
         <v>1000000</v>
       </c>
-      <c r="N47" s="10" t="s">
+      <c r="N47" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="O47" s="10" t="s">
+      <c r="O47" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="P47" s="10" t="s">
+      <c r="P47" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="R47" s="10">
+      <c r="R47" s="6">
         <v>1000000</v>
       </c>
-      <c r="S47" s="10">
+      <c r="S47" s="6">
         <v>63.661099999999998</v>
       </c>
-      <c r="T47" s="10" t="s">
+      <c r="T47" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="U47" s="10" t="s">
+      <c r="U47" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2996,6 +2992,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="D3:G4" formulaRange="1"/>
     <ignoredError sqref="D5:G7 E8:G8" evalError="1" formulaRange="1"/>

</xml_diff>